<commit_message>
modification template: ajout des champs commentaire et statut dans l'export
</commit_message>
<xml_diff>
--- a/src/main/resources/template-segur-requirement-export-avec-colonnes-prepub-modifie.xlsx
+++ b/src/main/resources/template-segur-requirement-export-avec-colonnes-prepub-modifie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flabatie\Documents\ENV-ANS\19-PLUGIN-SQUASH\squash-plugin\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379629DE-B3B9-4FF0-9B8D-C2B00458989C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2D3EF-0E0F-4D16-B3CB-214D352B221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Profil</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Exigence</t>
+  </si>
+  <si>
+    <t>Statut publication</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
   </si>
 </sst>
 </file>
@@ -707,11 +713,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15.5"/>
@@ -743,15 +749,15 @@
     <col min="25" max="25" width="18.5703125" style="7" customWidth="1"/>
     <col min="26" max="26" width="30.5703125" style="6" customWidth="1"/>
     <col min="27" max="27" width="18.5703125" style="7" customWidth="1"/>
-    <col min="28" max="28" width="30.5703125" style="6" customWidth="1"/>
-    <col min="29" max="32" width="15.2109375" style="21" customWidth="1"/>
-    <col min="33" max="33" width="40.28515625" style="21" customWidth="1"/>
-    <col min="34" max="34" width="52.28515625" style="21" customWidth="1"/>
-    <col min="35" max="35" width="13.92578125" style="21" customWidth="1"/>
-    <col min="36" max="16384" width="9.28515625" style="8"/>
+    <col min="28" max="30" width="30.5703125" style="6" customWidth="1"/>
+    <col min="31" max="34" width="15.2109375" style="21" customWidth="1"/>
+    <col min="35" max="35" width="40.28515625" style="21" customWidth="1"/>
+    <col min="36" max="36" width="52.28515625" style="21" customWidth="1"/>
+    <col min="37" max="37" width="13.92578125" style="21" customWidth="1"/>
+    <col min="38" max="16384" width="9.28515625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="56.25" customHeight="1">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="56.25" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>43</v>
       </c>
@@ -836,29 +842,35 @@
       <c r="AB1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AC1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AG1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="23" t="s">
+      <c r="AH1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="23" t="s">
+      <c r="AI1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="23" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AK1" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="21" customFormat="1" ht="68.25" customHeight="1">
+    <row r="2" spans="1:37" s="21" customFormat="1" ht="68.25" customHeight="1">
       <c r="A2" s="22" t="s">
         <v>36</v>
       </c>
@@ -943,30 +955,32 @@
       <c r="AB2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="19" t="s">
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF2" s="19" t="s">
+      <c r="AG2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK2" s="20" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:AB2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="AD2" r:id="rId1" xr:uid="{469CC100-57DA-4667-A398-7625D4E1EA7C}"/>
-    <hyperlink ref="AE2" r:id="rId2" xr:uid="{E89A2FEC-0659-4F61-ADA4-07A73EB5618E}"/>
-    <hyperlink ref="AF2" r:id="rId3" xr:uid="{4F8A1E68-C5B6-42D4-A495-3784461637C1}"/>
+    <hyperlink ref="AF2" r:id="rId1" xr:uid="{469CC100-57DA-4667-A398-7625D4E1EA7C}"/>
+    <hyperlink ref="AG2" r:id="rId2" xr:uid="{E89A2FEC-0659-4F61-ADA4-07A73EB5618E}"/>
+    <hyperlink ref="AH2" r:id="rId3" xr:uid="{4F8A1E68-C5B6-42D4-A495-3784461637C1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>